<commit_message>
LLM function v2 - Ok
</commit_message>
<xml_diff>
--- a/output_llm_change_analysis.xlsx
+++ b/output_llm_change_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oussa/Desktop/Github_perso/3 - Legal FR Tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17A0564-C656-8B42-A81E-4ADBBD7E98A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3882C3BD-0FE5-A544-9AA9-4C5754B22143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="740" windowWidth="29160" windowHeight="12160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="740" yWindow="740" windowWidth="28660" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -496,13 +496,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -810,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U2" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView tabSelected="1" topLeftCell="U3" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1014,68 +1017,68 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+    <row r="4" spans="1:22" s="2" customFormat="1" ht="338" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
         <v>690</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>2020</v>
       </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="b">
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="I4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="P4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="P4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="U4" t="s">
+      <c r="U4" s="2" t="s">
         <v>103</v>
       </c>
     </row>

</xml_diff>